<commit_message>
added config file and term highlighting
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HelpHub\Desktop\xendra-cards-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C153CFC-9CD9-4740-A648-17D125A4C705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE737F7C-9AD9-4C8F-9641-06111469AD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,32 +102,6 @@
     <t>Derribo</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Conjura este efecto para obtener todos los objetos sueltos en el área y provocar </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>electrificar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a los oponentes. También puedes activar los mecanismos. Además, puedes mover dentro de esta área (por teletransportación) tus trampas (mágicas o mecánicas) y Xendras.</t>
-    </r>
-  </si>
-  <si>
     <t>Asalto Magnético</t>
   </si>
   <si>
@@ -153,13 +127,18 @@
   </si>
   <si>
     <t>Instantáneo y más largo</t>
+  </si>
+  <si>
+    <t>Coloca esta trampa en un casillero desocupado. Bloquea de sus 8 direcciones una por cada nivel que tengas. Al ser pisado teletransporta al objetivo, trampa o proyectil a un casillero al azar: d8 dirección d6 distancia (cuenta en diagonal).
+Puedes seleccionar esta trampa para colocar otras trampas, efectos o habilidades no melé y estas se teletransportarán también.
+Al final de tu turno puedes modificar los bloqueos. Xendra.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,14 +148,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -213,6 +184,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,9 +587,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -623,25 +597,25 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -650,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -659,10 +633,10 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed colors, highlighting and modals
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,56 +436,59 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>range</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>area</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>worth</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>delay</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>effect</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>effect_type</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Amnesia</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Global</t>
@@ -493,83 +496,89 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Escoge entre una habilidad, ataque básico, conjurar, reposición o abrir Xendras y bloquea esta acción para el oponente durante 3 turnos.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Una acción</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Aturdir</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Penalizador</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Alimenta la bestia</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Objetivo</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Todo el daño recibido a partir de ahora y hasta el final del turno oponente, o hasta atacar, se suma a tu próximo ataque.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Una acción</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Instantáneo</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Aumento</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Bonificador</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Arenas movedizas</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>Global</t>
@@ -577,41 +586,44 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Coloca esta trampa sobre un casillero desocupado y crea un área donde desplazarse cuesta el doble para el oponente, es decir, antes de abandonar un casillero debe dar un paso nulo en el mismo.</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Coloca esta trampa sobre un casillero desocupado y crea un área donde desplazarse cuesta el doble para el oponente, es decir, antes de abandonar un casillero debe dar un paso nulo en el mismo. @asde</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Una acción</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Derribo</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Requiere ficha superficial</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Asalto Magnético</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>Global</t>
@@ -619,41 +631,44 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Coloca esta trampa en un casillero desocupado. Aplica @test_effect para después poder usar (@long_test_effect, está entre paréntesis para probar). El resto es una prueba  para saber hasta donde llega el texto, y tal vez un poquito más también (más que nada para probar la otra fuente). Esto ya es boludear porque necesito más caracteres. @thunder_storm no es @test_effect</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Una acción pero larga</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Instantáneo y más largo</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>No requiere prueba</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Levanta objetos a distancia</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Atrapa hechizos</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Global</t>
@@ -661,21 +676,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Limpia al objetivo de todo efecto mágico y modificador que esté actuando dentro de él y lo atrapa en este conjuro. Luego, aplica estos efectos sobre un objetivo como acción normal sin necesidad de prueba.</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Energizar</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Limpia efectos</t>
         </is>

</xml_diff>